<commit_message>
Bug fixes, network fixes, collision improvements
-Added more comments and fixed more messages
-Issues when player leaves, he is not properly deleted. Will need to add
more test players.
-Fixed more message pointers
-Noooooo not serverside logic
-Fixed and commented the maingame setup
-Worked on collisions between players in main game
-Fixed collision information in runClientLanMenu
-Commented some code in functions
-Added collision type field to player
-Fixed sending player information
-Added collisions between every player when the game has started
-Players not registering collision
-Issue with player location when starting game, it doesn't send some
movement data.
</commit_message>
<xml_diff>
--- a/Sendcodes.xlsx
+++ b/Sendcodes.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Looking for hosts (Client)</t>
   </si>
@@ -51,7 +50,31 @@
     <t>Adjust host ping</t>
   </si>
   <si>
-    <t>Movement info from server</t>
+    <t>Movement info from clients</t>
+  </si>
+  <si>
+    <t>Send a message to host that the client is still in the lobby</t>
+  </si>
+  <si>
+    <t>Add a new message to the chat box (client side)</t>
+  </si>
+  <si>
+    <t>Update player locations (client side)</t>
+  </si>
+  <si>
+    <t>Server gets a chat message and sends it to all of the players</t>
+  </si>
+  <si>
+    <t>Server recieves notice that the player is still in the lobby</t>
+  </si>
+  <si>
+    <t>Setup game for client</t>
+  </si>
+  <si>
+    <t>Delete a player that has left</t>
+  </si>
+  <si>
+    <t>Player has told server that he is leaving, tell rest of players</t>
   </si>
 </sst>
 </file>
@@ -372,7 +395,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,40 +468,64 @@
       <c r="A9">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>